<commit_message>
Incorporated new gas price data, and plotted results with lm
</commit_message>
<xml_diff>
--- a/data/external/fuel/fuel_emissions/EU-ETS-emission-factors-calorific-values-2017.xlsx
+++ b/data/external/fuel/fuel_emissions/EU-ETS-emission-factors-calorific-values-2017.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FBEAC4-74C8-D949-AE67-F1417F9864AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="923" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="923" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="311">
   <si>
     <t>Final Spreadsheet</t>
   </si>
@@ -1121,11 +1122,17 @@
   <si>
     <t>Average:</t>
   </si>
+  <si>
+    <t>t C per tonne consumed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$-809]dddd&quot;, &quot;mmmm&quot; &quot;dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -2274,6 +2281,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2289,36 +2314,18 @@
     <xf numFmtId="2" fontId="24" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="cf1" xfId="1"/>
-    <cellStyle name="cf2" xfId="2"/>
+    <cellStyle name="cf1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="cf2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="External" xfId="4"/>
+    <cellStyle name="External" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal_DAT33-2005_CEF_SummaryTable" xfId="6"/>
-    <cellStyle name="Normal_DAT33-2005_CEF_SummaryTable 2" xfId="7"/>
-    <cellStyle name="Normal_Extract" xfId="8"/>
-    <cellStyle name="Normal_Sheet3_1" xfId="9"/>
+    <cellStyle name="Normal_DAT33-2005_CEF_SummaryTable" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal_DAT33-2005_CEF_SummaryTable 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal_Extract" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal_Sheet3_1" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5738,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M89"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -5779,36 +5786,36 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="71.25" customHeight="1">
-      <c r="B9" s="218" t="s">
+      <c r="B9" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="218"/>
-      <c r="D9" s="218"/>
-      <c r="E9" s="218"/>
-      <c r="F9" s="218"/>
-      <c r="G9" s="218"/>
-      <c r="H9" s="218"/>
+      <c r="C9" s="224"/>
+      <c r="D9" s="224"/>
+      <c r="E9" s="224"/>
+      <c r="F9" s="224"/>
+      <c r="G9" s="224"/>
+      <c r="H9" s="224"/>
     </row>
     <row r="10" spans="2:13" ht="60.75" customHeight="1">
-      <c r="B10" s="218" t="s">
+      <c r="B10" s="224" t="s">
         <v>293</v>
       </c>
-      <c r="C10" s="218"/>
-      <c r="D10" s="218"/>
-      <c r="E10" s="218"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
+      <c r="C10" s="224"/>
+      <c r="D10" s="224"/>
+      <c r="E10" s="224"/>
+      <c r="F10" s="224"/>
+      <c r="G10" s="224"/>
+      <c r="H10" s="224"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1">
-      <c r="B11" s="219" t="s">
+      <c r="B11" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="219"/>
-      <c r="D11" s="219"/>
-      <c r="E11" s="219"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
+      <c r="C11" s="225"/>
+      <c r="D11" s="225"/>
+      <c r="E11" s="225"/>
+      <c r="F11" s="225"/>
+      <c r="G11" s="225"/>
     </row>
     <row r="12" spans="2:13" ht="18" customHeight="1">
       <c r="B12" t="s">
@@ -5976,16 +5983,16 @@
       <c r="I38" s="11"/>
     </row>
     <row r="39" spans="2:9">
-      <c r="B39" s="220" t="s">
+      <c r="B39" s="226" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="220"/>
-      <c r="D39" s="220"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
+      <c r="C39" s="226"/>
+      <c r="D39" s="226"/>
+      <c r="E39" s="226"/>
+      <c r="F39" s="226"/>
+      <c r="G39" s="226"/>
+      <c r="H39" s="226"/>
+      <c r="I39" s="226"/>
     </row>
     <row r="40" spans="2:9">
       <c r="B40" s="205" t="s">
@@ -6039,13 +6046,13 @@
       </c>
     </row>
     <row r="47" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B47" s="219"/>
-      <c r="C47" s="219"/>
-      <c r="D47" s="219"/>
-      <c r="E47" s="219"/>
-      <c r="F47" s="219"/>
-      <c r="G47" s="219"/>
-      <c r="H47" s="219"/>
+      <c r="B47" s="225"/>
+      <c r="C47" s="225"/>
+      <c r="D47" s="225"/>
+      <c r="E47" s="225"/>
+      <c r="F47" s="225"/>
+      <c r="G47" s="225"/>
+      <c r="H47" s="225"/>
     </row>
     <row r="49" spans="2:3">
       <c r="B49" s="2" t="s">
@@ -6300,11 +6307,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AJ99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="13"/>
@@ -6338,31 +6345,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="18">
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="227" t="s">
         <v>266</v>
       </c>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="221"/>
-      <c r="O2" s="221"/>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="221"/>
-      <c r="R2" s="221"/>
-      <c r="S2" s="221"/>
-      <c r="T2" s="221"/>
-      <c r="U2" s="221"/>
-      <c r="V2" s="221"/>
-      <c r="W2" s="221"/>
-      <c r="X2" s="221"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="227"/>
+      <c r="I2" s="227"/>
+      <c r="J2" s="227"/>
+      <c r="K2" s="227"/>
+      <c r="L2" s="227"/>
+      <c r="M2" s="227"/>
+      <c r="N2" s="227"/>
+      <c r="O2" s="227"/>
+      <c r="P2" s="227"/>
+      <c r="Q2" s="227"/>
+      <c r="R2" s="227"/>
+      <c r="S2" s="227"/>
+      <c r="T2" s="227"/>
+      <c r="U2" s="227"/>
+      <c r="V2" s="227"/>
+      <c r="W2" s="227"/>
+      <c r="X2" s="227"/>
     </row>
     <row r="3" spans="2:24" ht="19" thickBot="1">
       <c r="C3" s="19"/>
@@ -6460,7 +6467,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="2:24" ht="16">
+    <row r="7" spans="2:24" ht="17">
       <c r="B7" s="37" t="s">
         <v>262</v>
       </c>
@@ -6482,7 +6489,7 @@
       <c r="R7" s="42"/>
       <c r="S7" s="43"/>
     </row>
-    <row r="8" spans="2:24" ht="16">
+    <row r="8" spans="2:24" ht="17">
       <c r="B8" s="44"/>
       <c r="C8" s="45" t="s">
         <v>82</v>
@@ -6504,7 +6511,7 @@
         <v>2.2313981338681669E-3</v>
       </c>
       <c r="I8" s="49" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J8" s="49">
         <f>H8*1000</f>
@@ -6536,7 +6543,7 @@
       </c>
       <c r="S8" s="43"/>
     </row>
-    <row r="9" spans="2:24" ht="16">
+    <row r="9" spans="2:24" ht="17">
       <c r="B9" s="44"/>
       <c r="C9" s="45" t="s">
         <v>82</v>
@@ -6558,7 +6565,7 @@
         <v>3.06992746711721E-3</v>
       </c>
       <c r="I9" s="49" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J9" s="49">
         <f t="shared" ref="J9:J13" si="1">H9*1000</f>
@@ -6590,7 +6597,7 @@
       </c>
       <c r="S9" s="56"/>
     </row>
-    <row r="10" spans="2:24" ht="16">
+    <row r="10" spans="2:24" ht="17">
       <c r="B10" s="44"/>
       <c r="C10" s="45" t="s">
         <v>82</v>
@@ -6612,7 +6619,7 @@
         <v>3.179E-3</v>
       </c>
       <c r="I10" s="49" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J10" s="49">
         <f t="shared" si="1"/>
@@ -6644,7 +6651,7 @@
       </c>
       <c r="S10" s="43"/>
     </row>
-    <row r="11" spans="2:24" ht="16">
+    <row r="11" spans="2:24" ht="17">
       <c r="B11" s="44"/>
       <c r="C11" s="45" t="s">
         <v>82</v>
@@ -6666,7 +6673,7 @@
         <v>3.2003450253686523E-3</v>
       </c>
       <c r="I11" s="49" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J11" s="49">
         <f t="shared" si="1"/>
@@ -6698,7 +6705,7 @@
       </c>
       <c r="S11" s="43"/>
     </row>
-    <row r="12" spans="2:24" ht="16">
+    <row r="12" spans="2:24" ht="17">
       <c r="B12" s="44"/>
       <c r="C12" s="45" t="s">
         <v>82</v>
@@ -6720,7 +6727,7 @@
         <v>3.1900000000000001E-3</v>
       </c>
       <c r="I12" s="49" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J12" s="49">
         <f t="shared" si="1"/>
@@ -6752,7 +6759,7 @@
       </c>
       <c r="S12" s="43"/>
     </row>
-    <row r="13" spans="2:24" ht="16">
+    <row r="13" spans="2:24" ht="17">
       <c r="B13" s="44"/>
       <c r="C13" s="45" t="s">
         <v>82</v>
@@ -6769,16 +6776,15 @@
       <c r="G13" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H13" s="49">
-        <f t="shared" si="0"/>
-        <v>3.3777022306576414E-4</v>
+      <c r="H13" s="49" t="s">
+        <v>310</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>306</v>
-      </c>
-      <c r="J13" s="49">
+        <v>309</v>
+      </c>
+      <c r="J13" s="49" t="e">
         <f t="shared" si="1"/>
-        <v>0.33777022306576415</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K13" s="49" t="s">
         <v>306</v>
@@ -6806,7 +6812,7 @@
       </c>
       <c r="S13" s="43"/>
     </row>
-    <row r="14" spans="2:24" ht="16">
+    <row r="14" spans="2:24" ht="17">
       <c r="B14" s="44"/>
       <c r="C14" s="45" t="s">
         <v>82</v>
@@ -6814,25 +6820,25 @@
       <c r="D14" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="222" t="s">
+      <c r="E14" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="222"/>
-      <c r="H14" s="222"/>
-      <c r="I14" s="222"/>
-      <c r="J14" s="222"/>
-      <c r="K14" s="222"/>
-      <c r="L14" s="222"/>
-      <c r="M14" s="222"/>
-      <c r="N14" s="222"/>
-      <c r="O14" s="222"/>
-      <c r="P14" s="222"/>
-      <c r="Q14" s="222"/>
-      <c r="R14" s="222"/>
+      <c r="F14" s="228"/>
+      <c r="G14" s="228"/>
+      <c r="H14" s="228"/>
+      <c r="I14" s="228"/>
+      <c r="J14" s="228"/>
+      <c r="K14" s="228"/>
+      <c r="L14" s="228"/>
+      <c r="M14" s="228"/>
+      <c r="N14" s="228"/>
+      <c r="O14" s="228"/>
+      <c r="P14" s="228"/>
+      <c r="Q14" s="228"/>
+      <c r="R14" s="228"/>
       <c r="S14" s="43"/>
     </row>
-    <row r="15" spans="2:24" ht="16">
+    <row r="15" spans="2:24" ht="17">
       <c r="B15" s="58"/>
       <c r="C15" s="45" t="s">
         <v>82</v>
@@ -6884,7 +6890,7 @@
       </c>
       <c r="S15" s="43"/>
     </row>
-    <row r="16" spans="2:24" ht="16">
+    <row r="16" spans="2:24" ht="17">
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
         <v>82</v>
@@ -6920,7 +6926,7 @@
       <c r="R16" s="55"/>
       <c r="S16" s="43"/>
     </row>
-    <row r="17" spans="2:36" ht="17" thickBot="1">
+    <row r="17" spans="2:36" ht="18" thickBot="1">
       <c r="B17" s="59"/>
       <c r="C17" s="60" t="s">
         <v>82</v>
@@ -6972,7 +6978,7 @@
       </c>
       <c r="S17" s="43"/>
     </row>
-    <row r="18" spans="2:36" ht="16">
+    <row r="18" spans="2:36" ht="17">
       <c r="B18" s="63" t="s">
         <v>91</v>
       </c>
@@ -6981,10 +6987,10 @@
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="39"/>
-      <c r="H18" s="223"/>
-      <c r="I18" s="223"/>
-      <c r="J18" s="223"/>
-      <c r="K18" s="223"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="218"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="218"/>
       <c r="L18" s="64"/>
       <c r="M18" s="51"/>
       <c r="N18" s="65"/>
@@ -6994,7 +7000,7 @@
       <c r="R18" s="66"/>
       <c r="S18" s="43"/>
     </row>
-    <row r="19" spans="2:36" ht="16">
+    <row r="19" spans="2:36" ht="34">
       <c r="B19" s="44"/>
       <c r="C19" s="67" t="s">
         <v>92</v>
@@ -7011,10 +7017,10 @@
       <c r="G19" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H19" s="223"/>
-      <c r="I19" s="223"/>
-      <c r="J19" s="223"/>
-      <c r="K19" s="223"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218"/>
+      <c r="J19" s="218"/>
+      <c r="K19" s="218"/>
       <c r="L19" s="51">
         <v>79.006736623762308</v>
       </c>
@@ -7038,7 +7044,7 @@
       </c>
       <c r="S19" s="43"/>
     </row>
-    <row r="20" spans="2:36" ht="16">
+    <row r="20" spans="2:36" ht="34">
       <c r="B20" s="68"/>
       <c r="C20" s="67" t="s">
         <v>92</v>
@@ -7055,10 +7061,10 @@
       <c r="G20" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H20" s="223"/>
-      <c r="I20" s="223"/>
-      <c r="J20" s="223"/>
-      <c r="K20" s="223"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218"/>
+      <c r="J20" s="218"/>
+      <c r="K20" s="218"/>
       <c r="L20" s="51">
         <v>74.937503780817948</v>
       </c>
@@ -7082,7 +7088,7 @@
       </c>
       <c r="S20" s="43"/>
     </row>
-    <row r="21" spans="2:36" ht="16">
+    <row r="21" spans="2:36" ht="34">
       <c r="B21" s="68"/>
       <c r="C21" s="67" t="s">
         <v>92</v>
@@ -7126,7 +7132,7 @@
       </c>
       <c r="S21" s="43"/>
     </row>
-    <row r="22" spans="2:36" ht="16">
+    <row r="22" spans="2:36" ht="34">
       <c r="B22" s="68"/>
       <c r="C22" s="67" t="s">
         <v>92</v>
@@ -7143,10 +7149,10 @@
       <c r="G22" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H22" s="223"/>
-      <c r="I22" s="223"/>
-      <c r="J22" s="223"/>
-      <c r="K22" s="223"/>
+      <c r="H22" s="218"/>
+      <c r="I22" s="218"/>
+      <c r="J22" s="218"/>
+      <c r="K22" s="218"/>
       <c r="L22" s="51">
         <v>68.930745772941563</v>
       </c>
@@ -7170,7 +7176,7 @@
       </c>
       <c r="S22" s="43"/>
     </row>
-    <row r="23" spans="2:36" ht="16">
+    <row r="23" spans="2:36" ht="34">
       <c r="B23" s="68"/>
       <c r="C23" s="67" t="s">
         <v>92</v>
@@ -7178,25 +7184,25 @@
       <c r="D23" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="222" t="s">
+      <c r="E23" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F23" s="222"/>
-      <c r="G23" s="222"/>
-      <c r="H23" s="222"/>
-      <c r="I23" s="222"/>
-      <c r="J23" s="222"/>
-      <c r="K23" s="222"/>
-      <c r="L23" s="222"/>
-      <c r="M23" s="222"/>
-      <c r="N23" s="222"/>
-      <c r="O23" s="222"/>
-      <c r="P23" s="222"/>
-      <c r="Q23" s="222"/>
-      <c r="R23" s="222"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="228"/>
+      <c r="H23" s="228"/>
+      <c r="I23" s="228"/>
+      <c r="J23" s="228"/>
+      <c r="K23" s="228"/>
+      <c r="L23" s="228"/>
+      <c r="M23" s="228"/>
+      <c r="N23" s="228"/>
+      <c r="O23" s="228"/>
+      <c r="P23" s="228"/>
+      <c r="Q23" s="228"/>
+      <c r="R23" s="228"/>
       <c r="S23" s="43"/>
     </row>
-    <row r="24" spans="2:36" ht="16">
+    <row r="24" spans="2:36" ht="34">
       <c r="B24" s="44"/>
       <c r="C24" s="67" t="s">
         <v>92</v>
@@ -7240,7 +7246,7 @@
       </c>
       <c r="S24" s="43"/>
     </row>
-    <row r="25" spans="2:36" ht="17" thickBot="1">
+    <row r="25" spans="2:36" ht="35" thickBot="1">
       <c r="B25" s="68"/>
       <c r="C25" s="70" t="s">
         <v>92</v>
@@ -7257,10 +7263,10 @@
       <c r="G25" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H25" s="223"/>
-      <c r="I25" s="223"/>
-      <c r="J25" s="223"/>
-      <c r="K25" s="223"/>
+      <c r="H25" s="218"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="218"/>
       <c r="L25" s="51">
         <v>100.37678087837044</v>
       </c>
@@ -7284,7 +7290,7 @@
       </c>
       <c r="S25" s="43"/>
     </row>
-    <row r="26" spans="2:36" s="17" customFormat="1" ht="16">
+    <row r="26" spans="2:36" s="17" customFormat="1" ht="17">
       <c r="B26" s="63" t="s">
         <v>95</v>
       </c>
@@ -7322,7 +7328,7 @@
       <c r="AH26" s="13"/>
       <c r="AI26" s="13"/>
     </row>
-    <row r="27" spans="2:36" s="17" customFormat="1" ht="32">
+    <row r="27" spans="2:36" s="17" customFormat="1" ht="34">
       <c r="B27" s="44"/>
       <c r="C27" s="67" t="s">
         <v>96</v>
@@ -7382,7 +7388,7 @@
       <c r="AH27" s="13"/>
       <c r="AI27" s="13"/>
     </row>
-    <row r="28" spans="2:36" s="17" customFormat="1" ht="33" thickBot="1">
+    <row r="28" spans="2:36" s="17" customFormat="1" ht="35" thickBot="1">
       <c r="B28" s="76"/>
       <c r="C28" s="70" t="s">
         <v>96</v>
@@ -7442,7 +7448,7 @@
       <c r="AH28" s="13"/>
       <c r="AI28" s="13"/>
     </row>
-    <row r="29" spans="2:36" ht="16">
+    <row r="29" spans="2:36" ht="17">
       <c r="B29" s="83" t="s">
         <v>99</v>
       </c>
@@ -7464,7 +7470,7 @@
       <c r="R29" s="55"/>
       <c r="S29" s="43"/>
     </row>
-    <row r="30" spans="2:36" ht="32">
+    <row r="30" spans="2:36" ht="34">
       <c r="B30" s="68"/>
       <c r="C30" s="87" t="s">
         <v>100</v>
@@ -7511,7 +7517,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="31" spans="2:36" ht="33" thickBot="1">
+    <row r="31" spans="2:36" ht="35" thickBot="1">
       <c r="B31" s="68"/>
       <c r="C31" s="87" t="s">
         <v>102</v>
@@ -7558,7 +7564,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="32" spans="2:36" s="17" customFormat="1" ht="16">
+    <row r="32" spans="2:36" s="17" customFormat="1" ht="17">
       <c r="B32" s="63" t="s">
         <v>103</v>
       </c>
@@ -7596,7 +7602,7 @@
       <c r="AH32" s="13"/>
       <c r="AI32" s="13"/>
     </row>
-    <row r="33" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="33" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B33" s="44"/>
       <c r="C33" s="45" t="s">
         <v>104</v>
@@ -7656,7 +7662,7 @@
       <c r="AH33" s="13"/>
       <c r="AI33" s="13"/>
     </row>
-    <row r="34" spans="2:35" ht="32">
+    <row r="34" spans="2:35" ht="34">
       <c r="B34" s="68"/>
       <c r="C34" s="45" t="s">
         <v>104</v>
@@ -7700,7 +7706,7 @@
       </c>
       <c r="S34" s="43"/>
     </row>
-    <row r="35" spans="2:35" ht="32">
+    <row r="35" spans="2:35" ht="34">
       <c r="B35" s="68"/>
       <c r="C35" s="45" t="s">
         <v>104</v>
@@ -7744,7 +7750,7 @@
       </c>
       <c r="S35" s="43"/>
     </row>
-    <row r="36" spans="2:35" ht="32">
+    <row r="36" spans="2:35" ht="34">
       <c r="B36" s="68"/>
       <c r="C36" s="45" t="s">
         <v>104</v>
@@ -7752,25 +7758,25 @@
       <c r="D36" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="222" t="s">
+      <c r="E36" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F36" s="222"/>
-      <c r="G36" s="222"/>
-      <c r="H36" s="222"/>
-      <c r="I36" s="222"/>
-      <c r="J36" s="222"/>
-      <c r="K36" s="222"/>
-      <c r="L36" s="222"/>
-      <c r="M36" s="222"/>
-      <c r="N36" s="222"/>
-      <c r="O36" s="222"/>
-      <c r="P36" s="222"/>
-      <c r="Q36" s="222"/>
-      <c r="R36" s="222"/>
+      <c r="F36" s="228"/>
+      <c r="G36" s="228"/>
+      <c r="H36" s="228"/>
+      <c r="I36" s="228"/>
+      <c r="J36" s="228"/>
+      <c r="K36" s="228"/>
+      <c r="L36" s="228"/>
+      <c r="M36" s="228"/>
+      <c r="N36" s="228"/>
+      <c r="O36" s="228"/>
+      <c r="P36" s="228"/>
+      <c r="Q36" s="228"/>
+      <c r="R36" s="228"/>
       <c r="S36" s="43"/>
     </row>
-    <row r="37" spans="2:35" ht="33" thickBot="1">
+    <row r="37" spans="2:35" ht="35" thickBot="1">
       <c r="B37" s="76"/>
       <c r="C37" s="45" t="s">
         <v>104</v>
@@ -7814,7 +7820,7 @@
       </c>
       <c r="S37" s="43"/>
     </row>
-    <row r="38" spans="2:35" ht="32">
+    <row r="38" spans="2:35" ht="34">
       <c r="B38" s="63" t="s">
         <v>105</v>
       </c>
@@ -7823,10 +7829,10 @@
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
       <c r="G38" s="91"/>
-      <c r="H38" s="224"/>
-      <c r="I38" s="224"/>
-      <c r="J38" s="224"/>
-      <c r="K38" s="224"/>
+      <c r="H38" s="219"/>
+      <c r="I38" s="219"/>
+      <c r="J38" s="219"/>
+      <c r="K38" s="219"/>
       <c r="L38" s="92"/>
       <c r="M38" s="89"/>
       <c r="N38" s="93"/>
@@ -7853,10 +7859,10 @@
       <c r="G39" s="94" t="s">
         <v>270</v>
       </c>
-      <c r="H39" s="225"/>
-      <c r="I39" s="225"/>
-      <c r="J39" s="225"/>
-      <c r="K39" s="225"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
+      <c r="K39" s="220"/>
       <c r="L39" s="95">
         <v>275.26244405708604</v>
       </c>
@@ -7880,7 +7886,7 @@
       </c>
       <c r="S39" s="43"/>
     </row>
-    <row r="40" spans="2:35" ht="16">
+    <row r="40" spans="2:35" ht="17">
       <c r="B40" s="68"/>
       <c r="C40" s="84" t="s">
         <v>106</v>
@@ -7897,10 +7903,10 @@
       <c r="G40" s="94" t="s">
         <v>270</v>
       </c>
-      <c r="H40" s="225"/>
-      <c r="I40" s="225"/>
-      <c r="J40" s="225"/>
-      <c r="K40" s="225"/>
+      <c r="H40" s="220"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
       <c r="L40" s="95">
         <v>43.483400128912734</v>
       </c>
@@ -7924,7 +7930,7 @@
       </c>
       <c r="S40" s="43"/>
     </row>
-    <row r="41" spans="2:35" ht="32">
+    <row r="41" spans="2:35" ht="34">
       <c r="B41" s="68"/>
       <c r="C41" s="84" t="s">
         <v>107</v>
@@ -7941,10 +7947,10 @@
       <c r="G41" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="H41" s="225"/>
-      <c r="I41" s="225"/>
-      <c r="J41" s="225"/>
-      <c r="K41" s="225"/>
+      <c r="H41" s="220"/>
+      <c r="I41" s="220"/>
+      <c r="J41" s="220"/>
+      <c r="K41" s="220"/>
       <c r="L41" s="95">
         <v>108.43968446192902</v>
       </c>
@@ -7968,7 +7974,7 @@
       </c>
       <c r="S41" s="56"/>
     </row>
-    <row r="42" spans="2:35" ht="32">
+    <row r="42" spans="2:35" ht="34">
       <c r="B42" s="97"/>
       <c r="C42" s="84" t="s">
         <v>107</v>
@@ -7985,10 +7991,10 @@
       <c r="G42" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="H42" s="225"/>
-      <c r="I42" s="225"/>
-      <c r="J42" s="225"/>
-      <c r="K42" s="225"/>
+      <c r="H42" s="220"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
+      <c r="K42" s="220"/>
       <c r="L42" s="95">
         <v>74.937503780817948</v>
       </c>
@@ -8012,7 +8018,7 @@
       </c>
       <c r="S42" s="43"/>
     </row>
-    <row r="43" spans="2:35" ht="33" thickBot="1">
+    <row r="43" spans="2:35" ht="35" thickBot="1">
       <c r="B43" s="97"/>
       <c r="C43" s="84" t="s">
         <v>107</v>
@@ -8029,10 +8035,10 @@
       <c r="G43" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="H43" s="225"/>
-      <c r="I43" s="225"/>
-      <c r="J43" s="225"/>
-      <c r="K43" s="225"/>
+      <c r="H43" s="220"/>
+      <c r="I43" s="220"/>
+      <c r="J43" s="220"/>
+      <c r="K43" s="220"/>
       <c r="L43" s="95">
         <v>79.070517395769954</v>
       </c>
@@ -8056,7 +8062,7 @@
       </c>
       <c r="S43" s="43"/>
     </row>
-    <row r="44" spans="2:35" ht="32">
+    <row r="44" spans="2:35" ht="34">
       <c r="B44" s="63" t="s">
         <v>105</v>
       </c>
@@ -8064,10 +8070,10 @@
       <c r="E44" s="50"/>
       <c r="F44" s="48"/>
       <c r="G44" s="94"/>
-      <c r="H44" s="225"/>
-      <c r="I44" s="225"/>
-      <c r="J44" s="225"/>
-      <c r="K44" s="225"/>
+      <c r="H44" s="220"/>
+      <c r="I44" s="220"/>
+      <c r="J44" s="220"/>
+      <c r="K44" s="220"/>
       <c r="L44" s="98"/>
       <c r="M44" s="50"/>
       <c r="N44" s="96"/>
@@ -8077,7 +8083,7 @@
       <c r="R44" s="55"/>
       <c r="S44" s="43"/>
     </row>
-    <row r="45" spans="2:35" ht="16">
+    <row r="45" spans="2:35" ht="17">
       <c r="B45" s="97"/>
       <c r="C45" s="84" t="s">
         <v>108</v>
@@ -8094,10 +8100,10 @@
       <c r="G45" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="H45" s="225"/>
-      <c r="I45" s="225"/>
-      <c r="J45" s="225"/>
-      <c r="K45" s="225"/>
+      <c r="H45" s="220"/>
+      <c r="I45" s="220"/>
+      <c r="J45" s="220"/>
+      <c r="K45" s="220"/>
       <c r="L45" s="95">
         <v>108.43968446192902</v>
       </c>
@@ -8121,7 +8127,7 @@
       </c>
       <c r="S45" s="56"/>
     </row>
-    <row r="46" spans="2:35" ht="16">
+    <row r="46" spans="2:35" ht="17">
       <c r="B46" s="99" t="s">
         <v>109</v>
       </c>
@@ -8130,10 +8136,10 @@
       <c r="E46" s="53"/>
       <c r="F46" s="53"/>
       <c r="G46" s="94"/>
-      <c r="H46" s="225"/>
-      <c r="I46" s="225"/>
-      <c r="J46" s="225"/>
-      <c r="K46" s="225"/>
+      <c r="H46" s="220"/>
+      <c r="I46" s="220"/>
+      <c r="J46" s="220"/>
+      <c r="K46" s="220"/>
       <c r="L46" s="98"/>
       <c r="M46" s="53"/>
       <c r="N46" s="96"/>
@@ -8143,7 +8149,7 @@
       <c r="R46" s="55"/>
       <c r="S46" s="43"/>
     </row>
-    <row r="47" spans="2:35" ht="16">
+    <row r="47" spans="2:35" ht="17">
       <c r="B47" s="101"/>
       <c r="C47" s="100" t="s">
         <v>110</v>
@@ -8160,10 +8166,10 @@
       <c r="G47" s="94" t="s">
         <v>270</v>
       </c>
-      <c r="H47" s="225"/>
-      <c r="I47" s="225"/>
-      <c r="J47" s="225"/>
-      <c r="K47" s="225"/>
+      <c r="H47" s="220"/>
+      <c r="I47" s="220"/>
+      <c r="J47" s="220"/>
+      <c r="K47" s="220"/>
       <c r="L47" s="95">
         <v>43.483400128912734</v>
       </c>
@@ -8187,7 +8193,7 @@
       </c>
       <c r="S47" s="43"/>
     </row>
-    <row r="48" spans="2:35" ht="16">
+    <row r="48" spans="2:35" ht="17">
       <c r="B48" s="99" t="s">
         <v>111</v>
       </c>
@@ -8196,10 +8202,10 @@
       <c r="E48" s="53"/>
       <c r="F48" s="53"/>
       <c r="G48" s="94"/>
-      <c r="H48" s="225"/>
-      <c r="I48" s="225"/>
-      <c r="J48" s="225"/>
-      <c r="K48" s="225"/>
+      <c r="H48" s="220"/>
+      <c r="I48" s="220"/>
+      <c r="J48" s="220"/>
+      <c r="K48" s="220"/>
       <c r="L48" s="95"/>
       <c r="M48" s="53"/>
       <c r="N48" s="96"/>
@@ -8209,7 +8215,7 @@
       <c r="R48" s="55"/>
       <c r="S48" s="43"/>
     </row>
-    <row r="49" spans="2:35" ht="17" thickBot="1">
+    <row r="49" spans="2:35" ht="18" thickBot="1">
       <c r="B49" s="103"/>
       <c r="C49" s="104" t="s">
         <v>110</v>
@@ -8226,10 +8232,10 @@
       <c r="G49" s="105" t="s">
         <v>270</v>
       </c>
-      <c r="H49" s="226"/>
-      <c r="I49" s="226"/>
-      <c r="J49" s="226"/>
-      <c r="K49" s="226"/>
+      <c r="H49" s="221"/>
+      <c r="I49" s="221"/>
+      <c r="J49" s="221"/>
+      <c r="K49" s="221"/>
       <c r="L49" s="106">
         <v>275.26244405708604</v>
       </c>
@@ -8253,7 +8259,7 @@
       </c>
       <c r="S49" s="43"/>
     </row>
-    <row r="50" spans="2:35" ht="32">
+    <row r="50" spans="2:35" ht="34">
       <c r="B50" s="37" t="s">
         <v>113</v>
       </c>
@@ -8262,10 +8268,10 @@
       <c r="E50" s="40"/>
       <c r="F50" s="53"/>
       <c r="G50" s="49"/>
-      <c r="H50" s="223"/>
-      <c r="I50" s="223"/>
-      <c r="J50" s="223"/>
-      <c r="K50" s="223"/>
+      <c r="H50" s="218"/>
+      <c r="I50" s="218"/>
+      <c r="J50" s="218"/>
+      <c r="K50" s="218"/>
       <c r="L50" s="109"/>
       <c r="M50" s="89"/>
       <c r="N50" s="72"/>
@@ -8275,7 +8281,7 @@
       <c r="R50" s="66"/>
       <c r="S50" s="43"/>
     </row>
-    <row r="51" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="51" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B51" s="44"/>
       <c r="C51" s="84" t="s">
         <v>114</v>
@@ -8292,10 +8298,10 @@
       <c r="G51" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H51" s="223"/>
-      <c r="I51" s="223"/>
-      <c r="J51" s="223"/>
-      <c r="K51" s="223"/>
+      <c r="H51" s="218"/>
+      <c r="I51" s="218"/>
+      <c r="J51" s="218"/>
+      <c r="K51" s="218"/>
       <c r="L51" s="51">
         <v>71.743925127849195</v>
       </c>
@@ -8335,7 +8341,7 @@
       <c r="AH51" s="13"/>
       <c r="AI51" s="13"/>
     </row>
-    <row r="52" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="52" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B52" s="44"/>
       <c r="C52" s="84" t="s">
         <v>114</v>
@@ -8352,10 +8358,10 @@
       <c r="G52" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H52" s="223"/>
-      <c r="I52" s="223"/>
-      <c r="J52" s="223"/>
-      <c r="K52" s="223"/>
+      <c r="H52" s="218"/>
+      <c r="I52" s="218"/>
+      <c r="J52" s="218"/>
+      <c r="K52" s="218"/>
       <c r="L52" s="51">
         <v>108.43968446192902</v>
       </c>
@@ -8395,7 +8401,7 @@
       <c r="AH52" s="13"/>
       <c r="AI52" s="13"/>
     </row>
-    <row r="53" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="53" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B53" s="44"/>
       <c r="C53" s="84" t="s">
         <v>114</v>
@@ -8455,7 +8461,7 @@
       <c r="AH53" s="13"/>
       <c r="AI53" s="13"/>
     </row>
-    <row r="54" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="54" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B54" s="44"/>
       <c r="C54" s="84" t="s">
         <v>114</v>
@@ -8515,7 +8521,7 @@
       <c r="AH54" s="13"/>
       <c r="AI54" s="13"/>
     </row>
-    <row r="55" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="55" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B55" s="44"/>
       <c r="C55" s="84" t="s">
         <v>114</v>
@@ -8532,10 +8538,10 @@
       <c r="G55" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="223"/>
-      <c r="I55" s="223"/>
-      <c r="J55" s="223"/>
-      <c r="K55" s="223"/>
+      <c r="H55" s="218"/>
+      <c r="I55" s="218"/>
+      <c r="J55" s="218"/>
+      <c r="K55" s="218"/>
       <c r="L55" s="51">
         <v>79.070517395769954</v>
       </c>
@@ -8575,7 +8581,7 @@
       <c r="AH55" s="13"/>
       <c r="AI55" s="13"/>
     </row>
-    <row r="56" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="56" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B56" s="44"/>
       <c r="C56" s="84" t="s">
         <v>114</v>
@@ -8592,10 +8598,10 @@
       <c r="G56" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H56" s="223"/>
-      <c r="I56" s="223"/>
-      <c r="J56" s="223"/>
-      <c r="K56" s="223"/>
+      <c r="H56" s="218"/>
+      <c r="I56" s="218"/>
+      <c r="J56" s="218"/>
+      <c r="K56" s="218"/>
       <c r="L56" s="51">
         <v>74.937503780817948</v>
       </c>
@@ -8635,7 +8641,7 @@
       <c r="AH56" s="13"/>
       <c r="AI56" s="13"/>
     </row>
-    <row r="57" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="57" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B57" s="44"/>
       <c r="C57" s="84" t="s">
         <v>114</v>
@@ -8695,7 +8701,7 @@
       <c r="AH57" s="13"/>
       <c r="AI57" s="13"/>
     </row>
-    <row r="58" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="58" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B58" s="44"/>
       <c r="C58" s="84" t="s">
         <v>114</v>
@@ -8712,10 +8718,10 @@
       <c r="G58" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H58" s="223"/>
-      <c r="I58" s="223"/>
-      <c r="J58" s="223"/>
-      <c r="K58" s="223"/>
+      <c r="H58" s="218"/>
+      <c r="I58" s="218"/>
+      <c r="J58" s="218"/>
+      <c r="K58" s="218"/>
       <c r="L58" s="51">
         <v>74.493168019335343</v>
       </c>
@@ -8755,7 +8761,7 @@
       <c r="AH58" s="13"/>
       <c r="AI58" s="13"/>
     </row>
-    <row r="59" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="59" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B59" s="44"/>
       <c r="C59" s="84" t="s">
         <v>114</v>
@@ -8763,22 +8769,22 @@
       <c r="D59" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="E59" s="222" t="s">
+      <c r="E59" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F59" s="222"/>
-      <c r="G59" s="222"/>
-      <c r="H59" s="222"/>
-      <c r="I59" s="222"/>
-      <c r="J59" s="222"/>
-      <c r="K59" s="222"/>
-      <c r="L59" s="222"/>
-      <c r="M59" s="222"/>
-      <c r="N59" s="222"/>
-      <c r="O59" s="222"/>
-      <c r="P59" s="222"/>
-      <c r="Q59" s="222"/>
-      <c r="R59" s="222"/>
+      <c r="F59" s="228"/>
+      <c r="G59" s="228"/>
+      <c r="H59" s="228"/>
+      <c r="I59" s="228"/>
+      <c r="J59" s="228"/>
+      <c r="K59" s="228"/>
+      <c r="L59" s="228"/>
+      <c r="M59" s="228"/>
+      <c r="N59" s="228"/>
+      <c r="O59" s="228"/>
+      <c r="P59" s="228"/>
+      <c r="Q59" s="228"/>
+      <c r="R59" s="228"/>
       <c r="S59" s="43"/>
       <c r="T59" s="13"/>
       <c r="U59" s="13"/>
@@ -8797,7 +8803,7 @@
       <c r="AH59" s="13"/>
       <c r="AI59" s="13"/>
     </row>
-    <row r="60" spans="2:35" s="17" customFormat="1" ht="64">
+    <row r="60" spans="2:35" s="17" customFormat="1" ht="68">
       <c r="B60" s="44"/>
       <c r="C60" s="84" t="s">
         <v>114</v>
@@ -8857,7 +8863,7 @@
       <c r="AH60" s="13"/>
       <c r="AI60" s="13"/>
     </row>
-    <row r="61" spans="2:35" s="17" customFormat="1" ht="65" thickBot="1">
+    <row r="61" spans="2:35" s="17" customFormat="1" ht="69" thickBot="1">
       <c r="B61" s="44"/>
       <c r="C61" s="60" t="s">
         <v>114</v>
@@ -8874,10 +8880,10 @@
       <c r="G61" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="H61" s="227"/>
-      <c r="I61" s="227"/>
-      <c r="J61" s="227"/>
-      <c r="K61" s="227"/>
+      <c r="H61" s="222"/>
+      <c r="I61" s="222"/>
+      <c r="J61" s="222"/>
+      <c r="K61" s="222"/>
       <c r="L61" s="79">
         <v>102.31955728246791</v>
       </c>
@@ -8917,7 +8923,7 @@
       <c r="AH61" s="13"/>
       <c r="AI61" s="13"/>
     </row>
-    <row r="62" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="62" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B62" s="37" t="s">
         <v>113</v>
       </c>
@@ -8926,10 +8932,10 @@
       <c r="E62" s="53"/>
       <c r="F62" s="53"/>
       <c r="G62" s="49"/>
-      <c r="H62" s="223"/>
-      <c r="I62" s="223"/>
-      <c r="J62" s="223"/>
-      <c r="K62" s="223"/>
+      <c r="H62" s="218"/>
+      <c r="I62" s="218"/>
+      <c r="J62" s="218"/>
+      <c r="K62" s="218"/>
       <c r="L62" s="64"/>
       <c r="M62" s="50"/>
       <c r="N62" s="74"/>
@@ -8972,10 +8978,10 @@
       <c r="G63" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H63" s="223"/>
-      <c r="I63" s="223"/>
-      <c r="J63" s="223"/>
-      <c r="K63" s="223"/>
+      <c r="H63" s="218"/>
+      <c r="I63" s="218"/>
+      <c r="J63" s="218"/>
+      <c r="K63" s="218"/>
       <c r="L63" s="51">
         <v>93.992174420405703</v>
       </c>
@@ -9024,10 +9030,10 @@
       <c r="E64" s="53"/>
       <c r="F64" s="48"/>
       <c r="G64" s="49"/>
-      <c r="H64" s="223"/>
-      <c r="I64" s="223"/>
-      <c r="J64" s="223"/>
-      <c r="K64" s="223"/>
+      <c r="H64" s="218"/>
+      <c r="I64" s="218"/>
+      <c r="J64" s="218"/>
+      <c r="K64" s="218"/>
       <c r="L64" s="51"/>
       <c r="M64" s="50"/>
       <c r="N64" s="74"/>
@@ -9070,10 +9076,10 @@
       <c r="G65" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H65" s="223"/>
-      <c r="I65" s="223"/>
-      <c r="J65" s="223"/>
-      <c r="K65" s="223"/>
+      <c r="H65" s="218"/>
+      <c r="I65" s="218"/>
+      <c r="J65" s="218"/>
+      <c r="K65" s="218"/>
       <c r="L65" s="51">
         <v>94.427594385354524</v>
       </c>
@@ -9130,10 +9136,10 @@
       <c r="G66" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H66" s="223"/>
-      <c r="I66" s="223"/>
-      <c r="J66" s="223"/>
-      <c r="K66" s="223"/>
+      <c r="H66" s="218"/>
+      <c r="I66" s="218"/>
+      <c r="J66" s="218"/>
+      <c r="K66" s="218"/>
       <c r="L66" s="51">
         <v>93.311403112373426</v>
       </c>
@@ -9190,10 +9196,10 @@
       <c r="G67" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H67" s="223"/>
-      <c r="I67" s="223"/>
-      <c r="J67" s="223"/>
-      <c r="K67" s="223"/>
+      <c r="H67" s="218"/>
+      <c r="I67" s="218"/>
+      <c r="J67" s="218"/>
+      <c r="K67" s="218"/>
       <c r="L67" s="51">
         <v>83.111868857472757</v>
       </c>
@@ -9250,10 +9256,10 @@
       <c r="G68" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H68" s="223"/>
-      <c r="I68" s="223"/>
-      <c r="J68" s="223"/>
-      <c r="K68" s="223"/>
+      <c r="H68" s="218"/>
+      <c r="I68" s="218"/>
+      <c r="J68" s="218"/>
+      <c r="K68" s="218"/>
       <c r="L68" s="51">
         <v>72.139999999999958</v>
       </c>
@@ -9310,10 +9316,10 @@
       <c r="G69" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H69" s="223"/>
-      <c r="I69" s="223"/>
-      <c r="J69" s="223"/>
-      <c r="K69" s="223"/>
+      <c r="H69" s="218"/>
+      <c r="I69" s="218"/>
+      <c r="J69" s="218"/>
+      <c r="K69" s="218"/>
       <c r="L69" s="51">
         <v>60.064098413355651</v>
       </c>
@@ -9370,10 +9376,10 @@
       <c r="G70" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H70" s="223"/>
-      <c r="I70" s="223"/>
-      <c r="J70" s="223"/>
-      <c r="K70" s="223"/>
+      <c r="H70" s="218"/>
+      <c r="I70" s="218"/>
+      <c r="J70" s="218"/>
+      <c r="K70" s="218"/>
       <c r="L70" s="51">
         <v>42.065724384241548</v>
       </c>
@@ -9435,7 +9441,7 @@
       <c r="R71" s="66"/>
       <c r="S71" s="43"/>
     </row>
-    <row r="72" spans="2:35" s="17" customFormat="1" ht="16">
+    <row r="72" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B72" s="44"/>
       <c r="C72" s="84" t="s">
         <v>121</v>
@@ -9452,10 +9458,10 @@
       <c r="G72" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H72" s="223"/>
-      <c r="I72" s="223"/>
-      <c r="J72" s="223"/>
-      <c r="K72" s="223"/>
+      <c r="H72" s="218"/>
+      <c r="I72" s="218"/>
+      <c r="J72" s="218"/>
+      <c r="K72" s="218"/>
       <c r="L72" s="51">
         <v>74.937503780817948</v>
       </c>
@@ -9495,7 +9501,7 @@
       <c r="AH72" s="13"/>
       <c r="AI72" s="13"/>
     </row>
-    <row r="73" spans="2:35" s="17" customFormat="1" ht="17" thickBot="1">
+    <row r="73" spans="2:35" s="17" customFormat="1" ht="35" thickBot="1">
       <c r="B73" s="76"/>
       <c r="C73" s="84" t="s">
         <v>121</v>
@@ -9512,10 +9518,10 @@
       <c r="G73" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="H73" s="223"/>
-      <c r="I73" s="223"/>
-      <c r="J73" s="223"/>
-      <c r="K73" s="223"/>
+      <c r="H73" s="218"/>
+      <c r="I73" s="218"/>
+      <c r="J73" s="218"/>
+      <c r="K73" s="218"/>
       <c r="L73" s="51">
         <v>69.98916722498025</v>
       </c>
@@ -9555,7 +9561,7 @@
       <c r="AH73" s="13"/>
       <c r="AI73" s="13"/>
     </row>
-    <row r="74" spans="2:35" s="17" customFormat="1" ht="16">
+    <row r="74" spans="2:35" s="17" customFormat="1" ht="17">
       <c r="B74" s="63" t="s">
         <v>123</v>
       </c>
@@ -9593,7 +9599,7 @@
       <c r="AH74" s="13"/>
       <c r="AI74" s="13"/>
     </row>
-    <row r="75" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="75" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B75" s="44"/>
       <c r="C75" s="45" t="s">
         <v>124</v>
@@ -9610,10 +9616,10 @@
       <c r="G75" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H75" s="223"/>
-      <c r="I75" s="223"/>
-      <c r="J75" s="223"/>
-      <c r="K75" s="223"/>
+      <c r="H75" s="218"/>
+      <c r="I75" s="218"/>
+      <c r="J75" s="218"/>
+      <c r="K75" s="218"/>
       <c r="L75" s="51">
         <v>95.017543147845515</v>
       </c>
@@ -9653,7 +9659,7 @@
       <c r="AH75" s="13"/>
       <c r="AI75" s="13"/>
     </row>
-    <row r="76" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="76" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B76" s="68"/>
       <c r="C76" s="45" t="s">
         <v>124</v>
@@ -9670,10 +9676,10 @@
       <c r="G76" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H76" s="223"/>
-      <c r="I76" s="223"/>
-      <c r="J76" s="223"/>
-      <c r="K76" s="223"/>
+      <c r="H76" s="218"/>
+      <c r="I76" s="218"/>
+      <c r="J76" s="218"/>
+      <c r="K76" s="218"/>
       <c r="L76" s="51">
         <v>79.070517395769954</v>
       </c>
@@ -9713,7 +9719,7 @@
       <c r="AH76" s="13"/>
       <c r="AI76" s="13"/>
     </row>
-    <row r="77" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="77" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B77" s="68"/>
       <c r="C77" s="45" t="s">
         <v>124</v>
@@ -9730,10 +9736,10 @@
       <c r="G77" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H77" s="223"/>
-      <c r="I77" s="223"/>
-      <c r="J77" s="223"/>
-      <c r="K77" s="223"/>
+      <c r="H77" s="218"/>
+      <c r="I77" s="218"/>
+      <c r="J77" s="218"/>
+      <c r="K77" s="218"/>
       <c r="L77" s="51">
         <v>74.937503780817948</v>
       </c>
@@ -9773,7 +9779,7 @@
       <c r="AH77" s="13"/>
       <c r="AI77" s="13"/>
     </row>
-    <row r="78" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="78" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B78" s="68"/>
       <c r="C78" s="45" t="s">
         <v>124</v>
@@ -9790,10 +9796,10 @@
       <c r="G78" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H78" s="223"/>
-      <c r="I78" s="223"/>
-      <c r="J78" s="223"/>
-      <c r="K78" s="223"/>
+      <c r="H78" s="218"/>
+      <c r="I78" s="218"/>
+      <c r="J78" s="218"/>
+      <c r="K78" s="218"/>
       <c r="L78" s="51">
         <v>50.368360135067725</v>
       </c>
@@ -9833,7 +9839,7 @@
       <c r="AH78" s="13"/>
       <c r="AI78" s="13"/>
     </row>
-    <row r="79" spans="2:35" s="17" customFormat="1" ht="32">
+    <row r="79" spans="2:35" s="17" customFormat="1" ht="34">
       <c r="B79" s="68"/>
       <c r="C79" s="45" t="s">
         <v>124</v>
@@ -9841,22 +9847,22 @@
       <c r="D79" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="E79" s="222" t="s">
+      <c r="E79" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F79" s="222"/>
-      <c r="G79" s="222"/>
-      <c r="H79" s="222"/>
-      <c r="I79" s="222"/>
-      <c r="J79" s="222"/>
-      <c r="K79" s="222"/>
-      <c r="L79" s="222"/>
-      <c r="M79" s="222"/>
-      <c r="N79" s="222"/>
-      <c r="O79" s="222"/>
-      <c r="P79" s="222"/>
-      <c r="Q79" s="222"/>
-      <c r="R79" s="222"/>
+      <c r="F79" s="228"/>
+      <c r="G79" s="228"/>
+      <c r="H79" s="228"/>
+      <c r="I79" s="228"/>
+      <c r="J79" s="228"/>
+      <c r="K79" s="228"/>
+      <c r="L79" s="228"/>
+      <c r="M79" s="228"/>
+      <c r="N79" s="228"/>
+      <c r="O79" s="228"/>
+      <c r="P79" s="228"/>
+      <c r="Q79" s="228"/>
+      <c r="R79" s="228"/>
       <c r="S79" s="43"/>
       <c r="T79" s="13"/>
       <c r="U79" s="13"/>
@@ -9875,7 +9881,7 @@
       <c r="AH79" s="13"/>
       <c r="AI79" s="13"/>
     </row>
-    <row r="80" spans="2:35" ht="32">
+    <row r="80" spans="2:35" ht="34">
       <c r="B80" s="44"/>
       <c r="C80" s="45" t="s">
         <v>124</v>
@@ -9886,10 +9892,10 @@
       <c r="E80" s="53"/>
       <c r="F80" s="53"/>
       <c r="G80" s="49"/>
-      <c r="H80" s="223"/>
-      <c r="I80" s="223"/>
-      <c r="J80" s="223"/>
-      <c r="K80" s="223"/>
+      <c r="H80" s="218"/>
+      <c r="I80" s="218"/>
+      <c r="J80" s="218"/>
+      <c r="K80" s="218"/>
       <c r="L80" s="64"/>
       <c r="M80" s="50"/>
       <c r="N80" s="74"/>
@@ -9901,7 +9907,7 @@
       <c r="R80" s="55"/>
       <c r="S80" s="43"/>
     </row>
-    <row r="81" spans="2:35" s="17" customFormat="1" ht="33" thickBot="1">
+    <row r="81" spans="2:35" s="17" customFormat="1" ht="35" thickBot="1">
       <c r="B81" s="68"/>
       <c r="C81" s="45" t="s">
         <v>124</v>
@@ -9918,10 +9924,10 @@
       <c r="G81" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H81" s="223"/>
-      <c r="I81" s="223"/>
-      <c r="J81" s="223"/>
-      <c r="K81" s="223"/>
+      <c r="H81" s="218"/>
+      <c r="I81" s="218"/>
+      <c r="J81" s="218"/>
+      <c r="K81" s="218"/>
       <c r="L81" s="51">
         <v>71.743925127849195</v>
       </c>
@@ -9961,7 +9967,7 @@
       <c r="AH81" s="13"/>
       <c r="AI81" s="13"/>
     </row>
-    <row r="82" spans="2:35" ht="16">
+    <row r="82" spans="2:35" ht="17">
       <c r="B82" s="63" t="s">
         <v>125</v>
       </c>
@@ -9983,7 +9989,7 @@
       <c r="R82" s="66"/>
       <c r="S82" s="43"/>
     </row>
-    <row r="83" spans="2:35" ht="48">
+    <row r="83" spans="2:35" ht="51">
       <c r="B83" s="68"/>
       <c r="C83" s="45" t="s">
         <v>126</v>
@@ -10000,10 +10006,10 @@
       <c r="G83" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H83" s="223"/>
-      <c r="I83" s="223"/>
-      <c r="J83" s="223"/>
-      <c r="K83" s="223"/>
+      <c r="H83" s="218"/>
+      <c r="I83" s="218"/>
+      <c r="J83" s="218"/>
+      <c r="K83" s="218"/>
       <c r="L83" s="51">
         <v>90.414618504195161</v>
       </c>
@@ -10027,7 +10033,7 @@
       </c>
       <c r="S83" s="43"/>
     </row>
-    <row r="84" spans="2:35" ht="16">
+    <row r="84" spans="2:35" ht="17">
       <c r="B84" s="68"/>
       <c r="C84" s="45" t="s">
         <v>127</v>
@@ -10044,10 +10050,10 @@
       <c r="G84" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H84" s="223"/>
-      <c r="I84" s="223"/>
-      <c r="J84" s="223"/>
-      <c r="K84" s="223"/>
+      <c r="H84" s="218"/>
+      <c r="I84" s="218"/>
+      <c r="J84" s="218"/>
+      <c r="K84" s="218"/>
       <c r="L84" s="51">
         <v>79.070517395769954</v>
       </c>
@@ -10071,7 +10077,7 @@
       </c>
       <c r="S84" s="43"/>
     </row>
-    <row r="85" spans="2:35" ht="16">
+    <row r="85" spans="2:35" ht="17">
       <c r="B85" s="68"/>
       <c r="C85" s="45" t="s">
         <v>127</v>
@@ -10088,10 +10094,10 @@
       <c r="G85" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H85" s="223"/>
-      <c r="I85" s="223"/>
-      <c r="J85" s="223"/>
-      <c r="K85" s="223"/>
+      <c r="H85" s="218"/>
+      <c r="I85" s="218"/>
+      <c r="J85" s="218"/>
+      <c r="K85" s="218"/>
       <c r="L85" s="51">
         <v>74.937503780817948</v>
       </c>
@@ -10115,7 +10121,7 @@
       </c>
       <c r="S85" s="43"/>
     </row>
-    <row r="86" spans="2:35" ht="16">
+    <row r="86" spans="2:35" ht="17">
       <c r="B86" s="68"/>
       <c r="C86" s="45" t="s">
         <v>127</v>
@@ -10123,25 +10129,25 @@
       <c r="D86" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="E86" s="222" t="s">
+      <c r="E86" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="F86" s="222"/>
-      <c r="G86" s="222"/>
-      <c r="H86" s="222"/>
-      <c r="I86" s="222"/>
-      <c r="J86" s="222"/>
-      <c r="K86" s="222"/>
-      <c r="L86" s="222"/>
-      <c r="M86" s="222"/>
-      <c r="N86" s="222"/>
-      <c r="O86" s="222"/>
-      <c r="P86" s="222"/>
-      <c r="Q86" s="222"/>
-      <c r="R86" s="222"/>
+      <c r="F86" s="228"/>
+      <c r="G86" s="228"/>
+      <c r="H86" s="228"/>
+      <c r="I86" s="228"/>
+      <c r="J86" s="228"/>
+      <c r="K86" s="228"/>
+      <c r="L86" s="228"/>
+      <c r="M86" s="228"/>
+      <c r="N86" s="228"/>
+      <c r="O86" s="228"/>
+      <c r="P86" s="228"/>
+      <c r="Q86" s="228"/>
+      <c r="R86" s="228"/>
       <c r="S86" s="43"/>
     </row>
-    <row r="87" spans="2:35" s="17" customFormat="1" ht="48">
+    <row r="87" spans="2:35" s="17" customFormat="1" ht="51">
       <c r="B87" s="97"/>
       <c r="C87" s="45" t="s">
         <v>129</v>
@@ -10158,10 +10164,10 @@
       <c r="G87" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H87" s="223"/>
-      <c r="I87" s="223"/>
-      <c r="J87" s="223"/>
-      <c r="K87" s="223"/>
+      <c r="H87" s="218"/>
+      <c r="I87" s="218"/>
+      <c r="J87" s="218"/>
+      <c r="K87" s="218"/>
       <c r="L87" s="51">
         <v>95.017543147845515</v>
       </c>
@@ -10201,7 +10207,7 @@
       <c r="AH87" s="13"/>
       <c r="AI87" s="13"/>
     </row>
-    <row r="88" spans="2:35" ht="49" thickBot="1">
+    <row r="88" spans="2:35" ht="52" thickBot="1">
       <c r="B88" s="76"/>
       <c r="C88" s="60" t="s">
         <v>129</v>
@@ -10218,10 +10224,10 @@
       <c r="G88" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="H88" s="227"/>
-      <c r="I88" s="227"/>
-      <c r="J88" s="227"/>
-      <c r="K88" s="227"/>
+      <c r="H88" s="222"/>
+      <c r="I88" s="222"/>
+      <c r="J88" s="222"/>
+      <c r="K88" s="222"/>
       <c r="L88" s="79">
         <v>71.743925127849195</v>
       </c>
@@ -10267,47 +10273,47 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="2:35" ht="78">
+    <row r="91" spans="2:35" ht="84">
       <c r="B91" s="198" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="92" spans="2:35" ht="26">
+    <row r="92" spans="2:35" ht="28">
       <c r="B92" s="198" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="93" spans="2:35" ht="39">
+    <row r="93" spans="2:35" ht="42">
       <c r="B93" s="199" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="94" spans="2:35" ht="52">
+    <row r="94" spans="2:35" ht="56">
       <c r="B94" s="199" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="95" spans="2:35" ht="52">
+    <row r="95" spans="2:35" ht="56">
       <c r="B95" s="199" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="96" spans="2:35" ht="26">
+    <row r="96" spans="2:35" ht="28">
       <c r="B96" s="200" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="78">
+    <row r="97" spans="2:2" ht="84">
       <c r="B97" s="200" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="26">
+    <row r="98" spans="2:2" ht="28">
       <c r="B98" s="200" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="78">
+    <row r="99" spans="2:2" ht="84">
       <c r="B99" s="200" t="s">
         <v>260</v>
       </c>
@@ -10332,7 +10338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -10411,7 +10417,7 @@
       <c r="C5" s="130" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="228" t="s">
+      <c r="D5" s="223" t="s">
         <v>135</v>
       </c>
       <c r="E5" s="130" t="s">
@@ -10960,7 +10966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -11201,7 +11207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -11366,7 +11372,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E19" r:id="rId1"/>
+    <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="88" fitToWidth="0" fitToHeight="0" orientation="landscape"/>
@@ -11375,7 +11381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G88"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
@@ -11393,7 +11399,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14" thickBot="1"/>
-    <row r="2" spans="2:7" ht="19" thickBot="1">
+    <row r="2" spans="2:7" ht="20" thickBot="1">
       <c r="B2" s="159" t="s">
         <v>73</v>
       </c>
@@ -11802,7 +11808,7 @@
       <c r="E30" s="162"/>
       <c r="F30" s="162"/>
     </row>
-    <row r="31" spans="2:6" ht="16">
+    <row r="31" spans="2:6" ht="17">
       <c r="B31" s="176"/>
       <c r="C31" s="87" t="s">
         <v>100</v>
@@ -11817,7 +11823,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="17" thickBot="1">
+    <row r="32" spans="2:6" ht="18" thickBot="1">
       <c r="B32" s="171"/>
       <c r="C32" s="87" t="s">
         <v>102</v>
@@ -12400,7 +12406,7 @@
       <c r="E72" s="162"/>
       <c r="F72" s="162"/>
     </row>
-    <row r="73" spans="2:6" ht="16">
+    <row r="73" spans="2:6" ht="17">
       <c r="B73" s="187"/>
       <c r="C73" s="45" t="s">
         <v>126</v>

</xml_diff>